<commit_message>
Updated graph with moving average
</commit_message>
<xml_diff>
--- a/contrib/vstudio/vc14/deflate_silicia_corpus txt_256.xlsx
+++ b/contrib/vstudio/vc14/deflate_silicia_corpus txt_256.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gbonneau\git\zlib\contrib\vstudio\vc14\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1506AAA8-F96D-4081-AB95-4DD702CE04F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49931977-B606-4B91-9E6C-92234B46EECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{7A9F576F-E896-4E25-9E8C-08E372920CD4}"/>
   </bookViews>
@@ -1126,7 +1126,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+              <a:rPr lang="en-US" sz="1400" b="1" i="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
@@ -1134,7 +1134,7 @@
               </a:rPr>
               <a:t>LZ4 Compression</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US">
+            <a:endParaRPr lang="en-US" sz="1400">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -1150,15 +1150,15 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+              <a:rPr lang="en-US" sz="1400" b="1" i="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Wikipedia Chunk Size = 4096</a:t>
+              <a:t>Silicia Corpus Chunk Size = 256</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US">
+            <a:endParaRPr lang="en-US" sz="1400">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -3191,7 +3191,7 @@
         <c:axId val="211361871"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="7"/>
+          <c:max val="15"/>
           <c:min val="0.9"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -13584,7 +13584,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C0ADCAFA-9FA5-46AF-8C99-FFA963607EA2}" name="lz4_silicia_corpus_txt_256" displayName="lz4_silicia_corpus_txt_256" ref="A1:C326" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:C326" xr:uid="{C0ADCAFA-9FA5-46AF-8C99-FFA963607EA2}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{F81C7A6E-1E91-4175-BE58-F57CAA7982B1}" uniqueName="1" name="Source File Name = " queryTableFieldId="1" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{F81C7A6E-1E91-4175-BE58-F57CAA7982B1}" uniqueName="1" name="Source File Name = " queryTableFieldId="1" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{5F440207-5629-4B8A-AE01-0FE35ABF046F}" uniqueName="2" name="Column1" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{4F764508-500B-4D0A-B47A-A46C69150412}" uniqueName="3" name="_1" queryTableFieldId="3"/>
   </tableColumns>
@@ -13596,7 +13596,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C9C7949A-34FA-410E-B757-43B417EA2F42}" name="deflate_silicia_corpus_txt_256" displayName="deflate_silicia_corpus_txt_256" ref="A1:D278" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:D278" xr:uid="{C9C7949A-34FA-410E-B757-43B417EA2F42}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{871D6AED-8BE2-49C8-836C-1B5540724181}" uniqueName="1" name="Source File Name = " queryTableFieldId="1" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{871D6AED-8BE2-49C8-836C-1B5540724181}" uniqueName="1" name="Source File Name = " queryTableFieldId="1" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{A6EC4F71-A67A-4DDF-970E-E310297158E1}" uniqueName="2" name="Column1" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{3EE6EE25-6731-485C-8142-888535C802E2}" uniqueName="3" name="_1" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{0A5FF34E-B4E0-4A8C-ADDB-2587246D0043}" uniqueName="4" name="_2" queryTableFieldId="4"/>
@@ -13905,7 +13905,7 @@
   <dimension ref="A1:C326"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA39" sqref="AA39"/>
+      <selection activeCell="P47" sqref="P47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17478,7 +17478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA815D1E-BA12-4B3B-B635-E3525A8E27DE}">
   <dimension ref="A1:D278"/>
   <sheetViews>
-    <sheetView topLeftCell="A226" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A277" sqref="A277:XFD277"/>
     </sheetView>
   </sheetViews>

</xml_diff>